<commit_message>
ugr updated with L3s
</commit_message>
<xml_diff>
--- a/code/UG_nonsocial_bin1.xlsx
+++ b/code/UG_nonsocial_bin1.xlsx
@@ -13,7 +13,655 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Irrev</t>
+  </si>
+  <si>
+    <t>Irrev2</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
   <si>
     <t>Irrev</t>
   </si>
@@ -76,7 +724,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C114"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="true"/>
@@ -86,13 +734,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>3</v>
+        <v>219</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2">
@@ -548,32 +1196,32 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>145.90599555555556</v>
+        <v>170.82792384615385</v>
       </c>
       <c r="B43" s="0">
-        <v>1.5611314444444444</v>
+        <v>1.2883361538461537</v>
       </c>
       <c r="C43" s="0">
-        <v>10641</v>
+        <v>10640</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>232.27643333333333</v>
+        <v>145.90599555555556</v>
       </c>
       <c r="B44" s="0">
-        <v>1.2124486666666667</v>
+        <v>1.5611314444444444</v>
       </c>
       <c r="C44" s="0">
-        <v>10642</v>
+        <v>10641</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>232.56297500000002</v>
+        <v>232.27643333333333</v>
       </c>
       <c r="B45" s="0">
-        <v>1.0952887499999999</v>
+        <v>1.2124486666666667</v>
       </c>
       <c r="C45" s="0">
         <v>10642</v>
@@ -581,21 +1229,21 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>226.20811666666665</v>
+        <v>232.56297500000002</v>
       </c>
       <c r="B46" s="0">
-        <v>1.6415506666666666</v>
+        <v>1.0952887499999999</v>
       </c>
       <c r="C46" s="0">
-        <v>10644</v>
+        <v>10642</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>213.35917500000002</v>
+        <v>226.20811666666665</v>
       </c>
       <c r="B47" s="0">
-        <v>1.2095348333333333</v>
+        <v>1.6415506666666666</v>
       </c>
       <c r="C47" s="0">
         <v>10644</v>
@@ -603,21 +1251,21 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>146.26314000000002</v>
+        <v>213.35917500000002</v>
       </c>
       <c r="B48" s="0">
-        <v>0.95585987500000003</v>
+        <v>1.2095348333333333</v>
       </c>
       <c r="C48" s="0">
-        <v>10647</v>
+        <v>10644</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>212.13773750000001</v>
+        <v>146.26314000000002</v>
       </c>
       <c r="B49" s="0">
-        <v>0.74553799999999992</v>
+        <v>0.95585987500000003</v>
       </c>
       <c r="C49" s="0">
         <v>10647</v>
@@ -625,21 +1273,21 @@
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>188.46087142857144</v>
+        <v>212.13773750000001</v>
       </c>
       <c r="B50" s="0">
-        <v>1.849800571428571</v>
+        <v>0.74553799999999992</v>
       </c>
       <c r="C50" s="0">
-        <v>10649</v>
+        <v>10647</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>258.06438749999995</v>
+        <v>188.46087142857144</v>
       </c>
       <c r="B51" s="0">
-        <v>1.336820125</v>
+        <v>1.849800571428571</v>
       </c>
       <c r="C51" s="0">
         <v>10649</v>
@@ -647,21 +1295,21 @@
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>229.4963875</v>
+        <v>258.06438749999995</v>
       </c>
       <c r="B52" s="0">
-        <v>1.6084032499999998</v>
+        <v>1.336820125</v>
       </c>
       <c r="C52" s="0">
-        <v>10652</v>
+        <v>10649</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>197.83103333333332</v>
+        <v>229.4963875</v>
       </c>
       <c r="B53" s="0">
-        <v>1.8572911111111112</v>
+        <v>1.6084032499999998</v>
       </c>
       <c r="C53" s="0">
         <v>10652</v>
@@ -669,21 +1317,21 @@
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>184.98035555555558</v>
+        <v>197.83103333333332</v>
       </c>
       <c r="B54" s="0">
-        <v>0.77765722222222222</v>
+        <v>1.8572911111111112</v>
       </c>
       <c r="C54" s="0">
-        <v>10656</v>
+        <v>10652</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>180.13279999999997</v>
+        <v>184.98035555555558</v>
       </c>
       <c r="B55" s="0">
-        <v>0.9743860909090909</v>
+        <v>0.77765722222222222</v>
       </c>
       <c r="C55" s="0">
         <v>10656</v>
@@ -691,21 +1339,21 @@
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>233.14562666666669</v>
+        <v>180.13279999999997</v>
       </c>
       <c r="B56" s="0">
-        <v>1.4005677999999999</v>
+        <v>0.9743860909090909</v>
       </c>
       <c r="C56" s="0">
-        <v>10657</v>
+        <v>10656</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>171.25294285714287</v>
+        <v>233.14562666666669</v>
       </c>
       <c r="B57" s="0">
-        <v>1.3116289999999999</v>
+        <v>1.4005677999999999</v>
       </c>
       <c r="C57" s="0">
         <v>10657</v>
@@ -713,21 +1361,21 @@
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>210.20723529411762</v>
+        <v>171.25294285714287</v>
       </c>
       <c r="B58" s="0">
-        <v>1.4151625882352938</v>
+        <v>1.3116289999999999</v>
       </c>
       <c r="C58" s="0">
-        <v>10659</v>
+        <v>10657</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>183.65872999999999</v>
+        <v>210.20723529411762</v>
       </c>
       <c r="B59" s="0">
-        <v>1.5283026</v>
+        <v>1.4151625882352938</v>
       </c>
       <c r="C59" s="0">
         <v>10659</v>
@@ -735,21 +1383,21 @@
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>185.29762307692306</v>
+        <v>183.65872999999999</v>
       </c>
       <c r="B60" s="0">
-        <v>1.923052538461538</v>
+        <v>1.5283026</v>
       </c>
       <c r="C60" s="0">
-        <v>10663</v>
+        <v>10659</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>219.15474166666669</v>
+        <v>185.29762307692306</v>
       </c>
       <c r="B61" s="0">
-        <v>1.5610626666666665</v>
+        <v>1.923052538461538</v>
       </c>
       <c r="C61" s="0">
         <v>10663</v>
@@ -757,21 +1405,21 @@
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>182.81364999999997</v>
+        <v>219.15474166666669</v>
       </c>
       <c r="B62" s="0">
-        <v>1.5162343125000002</v>
+        <v>1.5610626666666665</v>
       </c>
       <c r="C62" s="0">
-        <v>10673</v>
+        <v>10663</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>219.1422583333333</v>
+        <v>182.81364999999997</v>
       </c>
       <c r="B63" s="0">
-        <v>0.96508033333333343</v>
+        <v>1.5162343125000002</v>
       </c>
       <c r="C63" s="0">
         <v>10673</v>
@@ -779,21 +1427,21 @@
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>184.99004444444444</v>
+        <v>219.1422583333333</v>
       </c>
       <c r="B64" s="0">
-        <v>1.9477473333333333</v>
+        <v>0.96508033333333343</v>
       </c>
       <c r="C64" s="0">
-        <v>10674</v>
+        <v>10673</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>224.71671111111112</v>
+        <v>184.99004444444444</v>
       </c>
       <c r="B65" s="0">
-        <v>1.3018891111111113</v>
+        <v>1.9477473333333333</v>
       </c>
       <c r="C65" s="0">
         <v>10674</v>
@@ -801,21 +1449,21 @@
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>165.42184615384616</v>
+        <v>224.71671111111112</v>
       </c>
       <c r="B66" s="0">
-        <v>1.3434256153846156</v>
+        <v>1.3018891111111113</v>
       </c>
       <c r="C66" s="0">
-        <v>10677</v>
+        <v>10674</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>204.61644166666667</v>
+        <v>165.42184615384616</v>
       </c>
       <c r="B67" s="0">
-        <v>1.3902820833333334</v>
+        <v>1.3434256153846156</v>
       </c>
       <c r="C67" s="0">
         <v>10677</v>
@@ -823,21 +1471,21 @@
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>184.51289166666666</v>
+        <v>204.61644166666667</v>
       </c>
       <c r="B68" s="0">
-        <v>1.6540624166666671</v>
+        <v>1.3902820833333334</v>
       </c>
       <c r="C68" s="0">
-        <v>10685</v>
+        <v>10677</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>219.90111666666667</v>
+        <v>184.51289166666666</v>
       </c>
       <c r="B69" s="0">
-        <v>1.3287584166666664</v>
+        <v>1.6540624166666671</v>
       </c>
       <c r="C69" s="0">
         <v>10685</v>
@@ -845,32 +1493,32 @@
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>237.08654999999999</v>
+        <v>219.90111666666667</v>
       </c>
       <c r="B70" s="0">
-        <v>1.2495490833333334</v>
+        <v>1.3287584166666664</v>
       </c>
       <c r="C70" s="0">
-        <v>10690</v>
+        <v>10685</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>212.45487499999999</v>
+        <v>237.08654999999999</v>
       </c>
       <c r="B71" s="0">
-        <v>1.7620562500000001</v>
+        <v>1.2495490833333334</v>
       </c>
       <c r="C71" s="0">
-        <v>10691</v>
+        <v>10690</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>219.85873333333333</v>
+        <v>212.45487499999999</v>
       </c>
       <c r="B72" s="0">
-        <v>1.4151924999999999</v>
+        <v>1.7620562500000001</v>
       </c>
       <c r="C72" s="0">
         <v>10691</v>
@@ -878,21 +1526,21 @@
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>230.81496250000001</v>
+        <v>219.85873333333333</v>
       </c>
       <c r="B73" s="0">
-        <v>1.2560401250000002</v>
+        <v>1.4151924999999999</v>
       </c>
       <c r="C73" s="0">
-        <v>10700</v>
+        <v>10691</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>210.18119999999999</v>
+        <v>230.81496250000001</v>
       </c>
       <c r="B74" s="0">
-        <v>1.059748066666667</v>
+        <v>1.2560401250000002</v>
       </c>
       <c r="C74" s="0">
         <v>10700</v>
@@ -900,21 +1548,21 @@
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>185.7602875</v>
+        <v>210.18119999999999</v>
       </c>
       <c r="B75" s="0">
-        <v>1.06025825</v>
+        <v>1.059748066666667</v>
       </c>
       <c r="C75" s="0">
-        <v>10701</v>
+        <v>10700</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>258.09201250000001</v>
+        <v>185.7602875</v>
       </c>
       <c r="B76" s="0">
-        <v>1.170582</v>
+        <v>1.06025825</v>
       </c>
       <c r="C76" s="0">
         <v>10701</v>
@@ -922,21 +1570,21 @@
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>185.74177500000002</v>
+        <v>258.09201250000001</v>
       </c>
       <c r="B77" s="0">
-        <v>0.99145362500000001</v>
+        <v>1.170582</v>
       </c>
       <c r="C77" s="0">
-        <v>10716</v>
+        <v>10701</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>258.04953749999999</v>
+        <v>185.74177500000002</v>
       </c>
       <c r="B78" s="0">
-        <v>0.97490549999999998</v>
+        <v>0.99145362500000001</v>
       </c>
       <c r="C78" s="0">
         <v>10716</v>
@@ -944,145 +1592,398 @@
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>185.76585</v>
+        <v>258.04953749999999</v>
       </c>
       <c r="B79" s="0">
-        <v>1.1018246250000001</v>
+        <v>0.97490549999999998</v>
       </c>
       <c r="C79" s="0">
-        <v>10720</v>
+        <v>10716</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>258.0567375</v>
+        <v>237.03885714285713</v>
       </c>
       <c r="B80" s="0">
-        <v>0.92704549999999997</v>
+        <v>1.3737693571428573</v>
       </c>
       <c r="C80" s="0">
-        <v>10720</v>
+        <v>10718</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>170.43465111111109</v>
+        <v>214.40835999999996</v>
       </c>
       <c r="B81" s="0">
-        <v>1.3184266666666666</v>
+        <v>1.5188336666666666</v>
       </c>
       <c r="C81" s="0">
-        <v>10741</v>
+        <v>10718</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>197.74928333333335</v>
+        <v>185.76585</v>
       </c>
       <c r="B82" s="0">
-        <v>1.1371544166666669</v>
+        <v>1.1018246250000001</v>
       </c>
       <c r="C82" s="0">
-        <v>10741</v>
+        <v>10720</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>188.35857333333334</v>
+        <v>258.0567375</v>
       </c>
       <c r="B83" s="0">
-        <v>0.98849833333333348</v>
+        <v>0.92704549999999997</v>
       </c>
       <c r="C83" s="0">
-        <v>10777</v>
+        <v>10720</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>180.06740375000001</v>
+        <v>170.43465111111109</v>
       </c>
       <c r="B84" s="0">
-        <v>1.1995782500000001</v>
+        <v>1.3184266666666666</v>
       </c>
       <c r="C84" s="0">
-        <v>10781</v>
+        <v>10741</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>186.83090000000001</v>
+        <v>197.74928333333335</v>
       </c>
       <c r="B85" s="0">
-        <v>1.1375332499999999</v>
+        <v>1.1371544166666669</v>
       </c>
       <c r="C85" s="0">
-        <v>10781</v>
+        <v>10741</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0">
-        <v>147.256124</v>
+        <v>200.01850000000002</v>
       </c>
       <c r="B86" s="0">
-        <v>1.8580616000000003</v>
+        <v>1.2966035454545457</v>
       </c>
       <c r="C86" s="0">
-        <v>10783</v>
+        <v>10767</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>199.63963636363636</v>
+        <v>188.18857999999997</v>
       </c>
       <c r="B87" s="0">
-        <v>1.2585852727272728</v>
+        <v>1.1295648888888887</v>
       </c>
       <c r="C87" s="0">
-        <v>10783</v>
+        <v>10770</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>196.51229999999998</v>
+        <v>114.67975777777777</v>
       </c>
       <c r="B88" s="0">
-        <v>1.2253861818181819</v>
+        <v>1.1278782222222221</v>
       </c>
       <c r="C88" s="0">
-        <v>10800</v>
+        <v>10770</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0">
-        <v>208.43698181818181</v>
+        <v>188.35857333333334</v>
       </c>
       <c r="B89" s="0">
-        <v>1.0848103636363635</v>
+        <v>0.98849833333333348</v>
       </c>
       <c r="C89" s="0">
-        <v>10800</v>
+        <v>10777</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>182.11470250000002</v>
+        <v>180.06740375000001</v>
       </c>
       <c r="B90" s="0">
-        <v>1.3917303750000001</v>
+        <v>1.1995782500000001</v>
       </c>
       <c r="C90" s="0">
-        <v>10804</v>
+        <v>10781</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0">
+        <v>186.83090000000001</v>
+      </c>
+      <c r="B91" s="0">
+        <v>1.1375332499999999</v>
+      </c>
+      <c r="C91" s="0">
+        <v>10781</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="0">
+        <v>147.256124</v>
+      </c>
+      <c r="B92" s="0">
+        <v>1.8580616000000003</v>
+      </c>
+      <c r="C92" s="0">
+        <v>10783</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="0">
+        <v>199.63963636363636</v>
+      </c>
+      <c r="B93" s="0">
+        <v>1.2585852727272728</v>
+      </c>
+      <c r="C93" s="0">
+        <v>10783</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="0">
+        <v>207.50008000000003</v>
+      </c>
+      <c r="B94" s="0">
+        <v>1.8879857999999998</v>
+      </c>
+      <c r="C94" s="0">
+        <v>10785</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="0">
+        <v>214.28395454545455</v>
+      </c>
+      <c r="B95" s="0">
+        <v>1.3540089090909091</v>
+      </c>
+      <c r="C95" s="0">
+        <v>10785</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="0">
+        <v>226.87047272727276</v>
+      </c>
+      <c r="B96" s="0">
+        <v>1.0011022727272729</v>
+      </c>
+      <c r="C96" s="0">
+        <v>10794</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0">
+        <v>172.33709166666668</v>
+      </c>
+      <c r="B97" s="0">
+        <v>0.8538629166666668</v>
+      </c>
+      <c r="C97" s="0">
+        <v>10794</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0">
+        <v>196.51229999999998</v>
+      </c>
+      <c r="B98" s="0">
+        <v>1.2253861818181819</v>
+      </c>
+      <c r="C98" s="0">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0">
+        <v>208.43698181818181</v>
+      </c>
+      <c r="B99" s="0">
+        <v>1.0848103636363635</v>
+      </c>
+      <c r="C99" s="0">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0">
+        <v>181.79063846153846</v>
+      </c>
+      <c r="B100" s="0">
+        <v>1.8254447692307691</v>
+      </c>
+      <c r="C100" s="0">
+        <v>10801</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0">
+        <v>202.79901785714284</v>
+      </c>
+      <c r="B101" s="0">
+        <v>1.6889194285714288</v>
+      </c>
+      <c r="C101" s="0">
+        <v>10801</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="0">
+        <v>162.04264285714285</v>
+      </c>
+      <c r="B102" s="0">
+        <v>1.5676196428571427</v>
+      </c>
+      <c r="C102" s="0">
+        <v>10802</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="0">
+        <v>187.53417142857143</v>
+      </c>
+      <c r="B103" s="0">
+        <v>1.2865482142857141</v>
+      </c>
+      <c r="C103" s="0">
+        <v>10802</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="0">
+        <v>196.93272000000005</v>
+      </c>
+      <c r="B104" s="0">
+        <v>1.0255111538461539</v>
+      </c>
+      <c r="C104" s="0">
+        <v>10803</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="0">
+        <v>182.11470250000002</v>
+      </c>
+      <c r="B105" s="0">
+        <v>1.3917303750000001</v>
+      </c>
+      <c r="C105" s="0">
+        <v>10804</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="0">
         <v>210.79172499999999</v>
       </c>
-      <c r="B91" s="0">
+      <c r="B106" s="0">
         <v>1.6373918750000003</v>
       </c>
-      <c r="C91" s="0">
+      <c r="C106" s="0">
         <v>10804</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="0">
+        <v>221.36985625000003</v>
+      </c>
+      <c r="B107" s="0">
+        <v>1.2945325624999997</v>
+      </c>
+      <c r="C107" s="0">
+        <v>10806</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="0">
+        <v>174.63843749999998</v>
+      </c>
+      <c r="B108" s="0">
+        <v>1.2539151874999996</v>
+      </c>
+      <c r="C108" s="0">
+        <v>10806</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="0">
+        <v>208.8583888888889</v>
+      </c>
+      <c r="B109" s="0">
+        <v>1.9736416666666667</v>
+      </c>
+      <c r="C109" s="0">
+        <v>10807</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="0">
+        <v>154.76408750000002</v>
+      </c>
+      <c r="B110" s="0">
+        <v>2.0433746250000002</v>
+      </c>
+      <c r="C110" s="0">
+        <v>10807</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="0">
+        <v>177.53695833333333</v>
+      </c>
+      <c r="B111" s="0">
+        <v>1.3264549999999999</v>
+      </c>
+      <c r="C111" s="0">
+        <v>10809</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="0">
+        <v>124.67671</v>
+      </c>
+      <c r="B112" s="0">
+        <v>1.0914141666666668</v>
+      </c>
+      <c r="C112" s="0">
+        <v>10809</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="0">
+        <v>172.90049999999999</v>
+      </c>
+      <c r="B113" s="0">
+        <v>1.6038641666666666</v>
+      </c>
+      <c r="C113" s="0">
+        <v>10812</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="0">
+        <v>136.46806666666666</v>
+      </c>
+      <c r="B114" s="0">
+        <v>1.5813845555555557</v>
+      </c>
+      <c r="C114" s="0">
+        <v>10812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>